<commit_message>
changes to Br and Cl to single character
</commit_message>
<xml_diff>
--- a/test_df_dror.xlsx
+++ b/test_df_dror.xlsx
@@ -28,7 +28,7 @@
     <t>N(C@[C-]@=O)C=C([C-]@=O)C=C(S)COCC00000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>OC=CC@ccOHccc(N(C)C)cCCCCCOHC@C(C@N)COHC[N+](C)C000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>OC=CC@cc&amp;ccc(N(C)C)cCCCCC&amp;C@C(C@N)C&amp;C[N+](C)C000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>OC(C=Nccncc(cNCCCC(CC#N)CC)C=CN)C000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
@@ -55,7 +55,7 @@
     <t>cccc(C[N+]CCN(C@C=C(C)N(CC)C(C@OCC)=CC)CC)cc0000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>Occcc(COcccOHccOHcC@C)cc000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>Occcc(COccc&amp;cc&amp;cC@C)cc00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>cccc(CC(C@NC(C@NCCCCC)Ccccc(OC[C-]@=O)c([C-]@=O)c)NC@CC[C-]@=O)cc0000000000000000000000000000000000000000000000000000000</t>
@@ -94,7 +94,7 @@
     <t>cccccc(NC@[C-]@=O)c([C-]@=O)ccc00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>Occcc(C@ccccOHccO)cOHc00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>Occcc(C@cccc&amp;ccO)c&amp;c0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>Occccc(-ccccc(CC([C-]@=O)[N+])c)c000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
@@ -109,7 +109,7 @@
     <t>Occcc(/C=C(\)[C-]@=O)cc0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>ccc(Cl)cc(Cn[c+](=N)nC(C)(C)C=O)c000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>ccc(l)cc(Cn[c+](=N)nC(C)(C)C=O)c0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>OCC[N+](CC)CCCOccccc(NC=NNC(CC@Nccccc(F)c)=C)ncncc0000000000000000000000000000000000000000000000000000000000000000000000</t>
@@ -118,7 +118,7 @@
     <t>OCCOC(NC=NC=CN=C(N)NC=O)CCO000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>Occcc(S@@ccccOHcc)cc0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>Occcc(S@@cccc&amp;cc)cc00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>CC@NCCCC[C-]@=O000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
@@ -148,7 +148,7 @@
     <t>NSN=C(CC([C-]@=O)[N+])C=O00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>cccc(C@N(ccccc(C=C(Br)C(OC[C-]@=O)=C([C-]@=O)S)c)CCCCCC)cc00000000000000000000000000000000000000000000000000000000000000</t>
+    <t>cccc(C@N(ccccc(C=C(*)C(OC[C-]@=O)=C([C-]@=O)S)c)CCCCCC)cc000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>ccc(NC)ccc-cccc(C)c(NCC@NS@=O)c00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
@@ -163,10 +163,10 @@
     <t>ccccc(c)-ccc(cccNCOC(C)(Ncccccc-)C(OC)C([N+]C)C)CNC=O0000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>OCCNC@cccc(C)c(NC@C(Cl)=C(OCcccc(F)ccF)N=C)c0000000000000000000000000000000000000000000000000000000000000000000000000000</t>
-  </si>
-  <si>
-    <t>cccc(ccCl)N=C([C-]@=O)CC=O0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>OCCNC@cccc(C)c(NC@C(l)=C(OCcccc(F)ccF)N=C)c00000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+  </si>
+  <si>
+    <t>cccc(ccl)N=C([C-]@=O)CC=O00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>NC@C=C(N(CC([C-]@=O)[N+])C=O)CCC0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
@@ -184,10 +184,10 @@
     <t>OC(CC(OCCOC)C@NC(C@NCcccccc)C(C)C)C(NC@ccc(C@NC(cccccc)C)cc(N(C)S@@C)c)COccc(F)cc(F)c00000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>/N=C\C=CN(COC(CO)COHCO)C@N0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
-  </si>
-  <si>
-    <t>OCCCC(C)C(C)CCOHCCCCC(C)C(C(C)CCC@NC[C-]@=O)CCC0000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>/N=C\C=CN(COC(CO)C&amp;CO)C@N00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+  </si>
+  <si>
+    <t>OCCCC(C)C(C)CC&amp;CCCCC(C)C(C(C)CCC@NC[C-]@=O)CCC00000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>OCC@CCCCCCC/C=C(\)C@CCC(C)CC@CCC0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
@@ -196,7 +196,7 @@
     <t>cnccc(-cc(-cccccccccc)nnc(N(C)C)c)c0000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>cccc(CS@@NCCC(Nccccc(C=C(Br)C(OC[C-]@=O)=C([C-]@=O)S)c)CC)cc000000000000000000000000000000000000000000000000000000000000</t>
+    <t>cccc(CS@@NCCC(Nccccc(C=C(*)C(OC[C-]@=O)=C([C-]@=O)S)c)CC)cc0000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>OCC(N/C=N\cc(N)ncnc)OCCOP@@OC0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
@@ -208,16 +208,16 @@
     <t>C=C(Ncnc(Scccc(NC@CCC)cc)nc(NCC[N+](C)CC)c)NN=CC000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>C=C(Cl)C@NC@NCC([C-]@=O)[N+]00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>C=C(l)C@NC@NCC([C-]@=O)[N+]000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>CCCCCCCCCCCCCCC[C-]@=O00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>cncc(-ccccc(C(CCC)C@n(C)[c+](=N)n)c)ccCl00000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
-  </si>
-  <si>
-    <t>C=C(ccncc(C#CC)c)SC(C(C)n[c+](=N)n(C)S@@C)=CCl00000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>cncc(-ccccc(C(CCC)C@n(C)[c+](=N)n)c)ccl000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+  </si>
+  <si>
+    <t>C=C(ccncc(C#CC)c)SC(C(C)n[c+](=N)n(C)S@@C)=Cl000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>Occcc(C)c(N(C@ccccc(C(F)(F)F)c)C=CN(C@C)cccccc)c000000000000000000000000000000000000000000000000000000000000000000000000</t>
@@ -238,16 +238,16 @@
     <t>C=CCCC=CCOccccc(C@CC@C@NCCN(C@C@CC@ccccc(OCCC=CC=CC)c)CC)c00000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>C=C(Br)C(OC[C-]@=O)=C([C-]@=O)S00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
-  </si>
-  <si>
-    <t>ccc(NC@Ncccc(Cl)c(Cl)c)cccCl00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>C=C(*)C(OC[C-]@=O)=C([C-]@=O)S000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+  </si>
+  <si>
+    <t>ccc(NC@Ncccc(l)c(l)c)cccl00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>OCC(CNC=N/C=C(C(C)C)C=NN/C(NCcccccc)=C\)CC[N+]C0000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>/C=C(\)N(C@C)/C=C\C=N/cccc(Cl)cc0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>/C=C(\)N(C@C)/C=C\C=N/cccc(l)cc00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>ccccc(c)-ccc(cccNCOC(Ncccccc-)CC)C@NC=O000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
@@ -259,7 +259,7 @@
     <t>C=C(C)CC(C[C-]@=O)C([C-]@=O)[N+]C000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>OC=C(ccccOHcc)OcccOHccOHcC=O00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>OC=C(cccc&amp;cc)Occc&amp;cc&amp;cC=O00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>C=CCCNC@ccnc(-ccc(C@NCCC)cccC)cc0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
@@ -268,7 +268,7 @@
     <t>cnccc(C=C(cccc(F)cc)NC(cccc(S@C)cc)=N)c000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>cccc(CC(Cl)[C-]@=O)cc000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>cccc(CC(l)[C-]@=O)cc0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>cnccc(-cc(-cccccccccc)nnc(NCC[N+]C(Ccccccc)C)c)c000000000000000000000000000000000000000000000000000000000000000000000000</t>
@@ -289,13 +289,13 @@
     <t>NC@NCC(CCCC[C-]@=O)SCC00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>OCC@NCCC(C=C(cncncc)C(cccc(Cl)cc)=NN)CC000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>OCC@NCCC(C=C(cncncc)C(cccc(l)cc)=NN)CC0000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>cccc(Nccccc(Ncccccc[C-]@=O)c[C-]@=O)c([C-]@=O)c0000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>OC=COHC(/COH=C(\)O)OCO00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>OC=C&amp;C(/C&amp;=C(\)O)OCO0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>OCCN(C@C(NC@C(C#N)CC)C(C)(C)C)C(C@NCcccc(C=C(C)N=CS)cc)C0000000000000000000000000000000000000000000000000000000000000000</t>
@@ -304,13 +304,13 @@
     <t>cccc(C(ccccc(-ccccc(OC)c)c)C@N(C)[c+](=N)n)cc000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>OC(C(NC@ccc(C@NC(cccccc)C)cc(N(C)S@@C)c)Ccccccc)C[N+]C(C@NCC(C)C)COHC000000000000000000000000000000000000000000000000000</t>
-  </si>
-  <si>
-    <t>cccc(CNccccc(C=C(Br)C(OC[C-]@=O)=C([C-]@=O)S)c)cc00000000000000000000000000000000000000000000000000000000000000000000000</t>
-  </si>
-  <si>
-    <t>Occ(Br)c(Br)c(Br)c(Br)cBr00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>OC(C(NC@ccc(C@NC(cccccc)C)cc(N(C)S@@C)c)Ccccccc)C[N+]C(C@NCC(C)C)C&amp;C0000000000000000000000000000000000000000000000000000</t>
+  </si>
+  <si>
+    <t>cccc(CNccccc(C=C(*)C(OC[C-]@=O)=C([C-]@=O)S)c)cc000000000000000000000000000000000000000000000000000000000000000000000000</t>
+  </si>
+  <si>
+    <t>Occ(*)c(*)c(*)c(*)c*0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>OCC(NC=Ncc(N)ncnc)OC(C[N+](Ccccc(F)cc)CCC([C-]@=O)[N+])CO000000000000000000000000000000000000000000000000000000000000000</t>
@@ -319,7 +319,7 @@
     <t>cc(OC)c(OC)cc(N)c[C-]@=O000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>cccc(ccCl)CNC@CN(C@C(CCCCCC)NC@CCNC@CO)CCC000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>cccc(ccl)CNC@CN(C@C(CCCCCC)NC@CCNC@CO)CCC0000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>CCC(C([C-]@=O)[N+])C[C-]@=O000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
@@ -337,10 +337,10 @@
     <t>C(=C(C(/)=C/ccccccC(C)CC)\C)/C=C/C(=C(\)[C-]@=O)C00000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>Occcc(/C=C(\)cccOHccOHc)c(Cl)c000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
-  </si>
-  <si>
-    <t>OCCOC(SCCCOHCOHC[N+]C)COHCOHCO000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>Occcc(/C=C(\)ccc&amp;cc&amp;c)c(l)c000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+  </si>
+  <si>
+    <t>OCCOC(SCCC&amp;C&amp;C[N+]C)C&amp;C&amp;CO0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>/C(=C(\)CCCCCCCC)CCCCCCC[C-]@=O00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
@@ -385,7 +385,7 @@
     <t>OCC(N/C=N\cc(N)ncnc)OC(COP@@OP@@=O)CO00000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>cnccncOCCCCCOcccc(Cl)ccNC@N000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>cnccncOCCCCCOcccc(l)ccNC@N0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>C(=C(C(/)=C/cccc(C)ccCCC)\C)/C=C/C(=C(\)[C-]@=O)C00000000000000000000000000000000000000000000000000000000000000000000000</t>
@@ -397,13 +397,13 @@
     <t>ccccc(c)C(OCCOCCC=CSC(NC@[C-]@=O)=C[C-]@=O)=NS@=O00000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>OCC@NC(C@NCCOHCCC@NCcccc(C=C(C)N=CS)cc)C(C)(C)C0000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>OCC@NC(C@NCC&amp;CCC@NCcccc(C=C(C)N=CS)cc)C(C)(C)C00000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>C(=C(C(/)=C/ccccccCCC)\C)/C=C/C(=C(\)[C-]@=O)C00000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>C=C(NC@Ncccc(Cl)cc)N(C)N=CC(C)(C)C00000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>C=C(NC@Ncccc(l)cc)N(C)N=CC(C)(C)C000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>C=CNC@cncnc(NCCCCCC)c000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
@@ -439,7 +439,7 @@
     <t>cnc(Nccccc(N@=O)c)nc(C=C(C)N=C(N)S)c000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>cccc(-cc([C-]@=O)c(NCCCCC)ncc(Cl)cc(Cl)cc)cc0000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>cccc(-cc([C-]@=O)c(NCCCCC)ncc(l)cc(l)cc)cc000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>cnc(Ncccc(S@@NCCOC)cc)nc(C=C(C)N(C)C@S)c00000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
@@ -454,7 +454,7 @@
     <t>C=Ncc(OCCCCCCC)nc(N)ncN0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>ccc(OCC@NCC)c(CNC@CN(C@C(CCCCCC)[N+])CCC)ccCl000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>ccc(OCC@NCC)c(CNC@CN(C@C(CCCCCC)[N+])CCC)ccl0000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>cccc(C(SC=NC=C(C@n[c+](=N)n)N)[C-]@=O)cc00000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
@@ -469,13 +469,13 @@
     <t>OCCN(C@C(NC@C)C(C)(C)C)C(C@NCcccc(C=C(C)N=CS)cc)CF0000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>cccc(C=C(Br)C(OC[C-]@=O)=C([C-]@=O)S)cc000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>cccc(C=C(*)C(OC[C-]@=O)=C([C-]@=O)S)cc0000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>Occcc([C-]@=O)ccF0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>OCCCOHCOHC[N+][N+]000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>OCCC&amp;C&amp;C[N+][N+]00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>cccc(Nccccccccc(S@@=O)c)cc0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
@@ -520,13 +520,13 @@
     <t>/C(C=N(C)ccccccC(C)C)=C(/)Ccccn(CCCS@@=O)cccccc0000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>cnc(Nccccc(Cl)cC)c([C-]@=O)cc0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
-  </si>
-  <si>
-    <t>OCOCCOHCOHCO000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
-  </si>
-  <si>
-    <t>ccc(C=C(Br)C(OC[C-]@=O)=C([C-]@=O)S)cc(N(C@NC)CCCCCC)c000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>cnc(Nccccc(l)cC)c([C-]@=O)cc00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+  </si>
+  <si>
+    <t>OCOCC&amp;C&amp;CO00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+  </si>
+  <si>
+    <t>ccc(C=C(*)C(OC[C-]@=O)=C([C-]@=O)S)cc(N(C@NC)CCCCCC)c0000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>cccccc(CCC@NCCCCCCC)c(N)ncc000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
@@ -544,7 +544,7 @@
     <t>C=CCC@NCCC([N+])CC000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>cc(N@=O)c(Cl)cc(CC([C-]@=O)[N+])cCC[C-]@=O000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>cc(N@=O)c(l)cc(CC([C-]@=O)[N+])cCC[C-]@=O0000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>/C(=C(/)CCCCCCCCCCC[C-]@=O)CC0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
@@ -556,7 +556,7 @@
     <t>C=C(NC@Nccccc(Ncncncccc(N)cc)c)N(cccc(C)cc)N=CC(C)(C)C000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>cccc(-cc([C-]@=O)c(NCCCCC)ncccc(Cl)cc)cc00000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>cccc(-cc([C-]@=O)c(NCCCCC)ncccc(l)cc)cc000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>Occcc(CC[N+])ccCCCCCC000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
@@ -568,7 +568,7 @@
     <t>C=CN(CC([C-]@=O)[N+])C@N(Ccccccc[C-]@=O)C=O00000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>Occc(CC(C@NCCCCOcccccOHcC@OC)NC@C)cccOC[C-]@=O00000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>Occc(CC(C@NCCCCOccccc&amp;cC@OC)NC@C)cccOC[C-]@=O000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>Occcccccc(N(C@[C-]@=O)cccccc[C-]@=O)cc0000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
@@ -583,7 +583,7 @@
     <t>OCCN(C@C(NC@C(NC@C)CC(C)C)C(C)(C)C)C(C@NCcccc(C=C(C)N=CS)cc)C00000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>Occcc(SccccOHcc)cc000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>Occcc(Scccc&amp;cc)cc0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>OCCN(C@ccccc(N)cC)C(C@NCcccc(C=C(C)N=CS)cc)C0000000000000000000000000000000000000000000000000000000000000000000000000000</t>
@@ -595,7 +595,7 @@
     <t>SCC(C@NCCCC[C-]@=O)C0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>ccc(Cl)cc(CNN=NC(C=C(CC([C-]@=O)[N+])C@NO)=N)c00000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>ccc(l)cc(CNN=NC(C=C(CC([C-]@=O)[N+])C@NO)=N)c000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>CC[N+]CCC([C-]@=O)[N+]00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
@@ -607,7 +607,7 @@
     <t>Occcc([C-]@=O)ccO0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>C=C(Cl)NC@C(=N)NC(Ccccccc)C[N+]CCC[N+]CCccccccCNC@C000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>C=C(l)NC@C(=N)NC(Ccccccc)C[N+]CCC[N+]CCccccccCNC@C0000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>N(C@OC)C=NN=C(SCC)S00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
@@ -634,34 +634,34 @@
     <t>cccc(CS@@NCCC(Nccccc(c)SC=CSC([C-]@=O)=COC[C-]@=O)CC)cc00000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>OCCOCOHCOHCOHCO000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>OCCOC&amp;C&amp;C&amp;CO000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>cccc(N(C@[C-]@=O)cccc(CC(C@NCCCCC)NS@@C)ccCCC@N)c([C-]@=O)c0000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>cccc(CS@@NCCC(Nccccc(C=C(Br)C(OC[C-]@=O)=C(C=NNN=N)S)c)CC)cc000000000000000000000000000000000000000000000000000000000000</t>
+    <t>cccc(CS@@NCCC(Nccccc(C=C(*)C(OC[C-]@=O)=C(C=NNN=N)S)c)CC)cc0000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>OCcc(cccc-ccccccNC(C)OC(Ncccccc-)CC([N+]C)COC)C@N00000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>Occ(Br)cc(/C=C/C@n[c+](=N)nC)ccBr000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
-  </si>
-  <si>
-    <t>ccc(C=C(Br)C(OC[C-]@=O)=C([C-]@=O)S)cc(NCCCCCC)c000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>Occ(*)cc(/C=C/C@n[c+](=N)nC)cc*00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+  </si>
+  <si>
+    <t>ccc(C=C(*)C(OC[C-]@=O)=C([C-]@=O)S)cc(NCCCCCC)c0000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>NOC(C)=C(CC([C-]@=O)[N+])C=O00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>cccc(-cc(C=NN=NN)c(NCCCCC)ncccc(Cl)cc)cc00000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>cccc(-cc(C=NN=NN)c(NCCCCC)ncccc(l)cc)cc000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>cnc(Ncccc(NCC[N+]CC)cc)nc(C=C(C)N(C)C@S)c0000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>Onc(NCC(F)(F)cccccnO)ccc(Cl)cCC@NC(ccccc(Cl)c)C0000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>Onc(NCC(F)(F)cccccnO)ccc(l)cCC@NC(ccccc(l)c)C000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>cccc(ccF)S@@NCNCCC000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
@@ -676,7 +676,7 @@
     <t>C=CC(CNC@C=CSC=CN(CC([C-]@=O)[N+])C=O)=C([C-]@=O)S0000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>C=NN(C)C@C(Br)/C=N/CCC(cccccc)C[N+](C)C000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>C=NN(C)C@C(*)/C=N/CCC(cccccc)C[N+](C)C0000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>SCCSCCSC(C)(C)C([C-]@=O)[N+]00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
@@ -712,7 +712,7 @@
     <t>NC@C=C(N(CC([C-]@=O)[N+])C=O)C[N+](C)C0000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>cc(Cl)c(Cl)nc(OC[C-]@=O)cCl000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>cc(l)c(l)nc(OC[C-]@=O)cl000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>Occccc(Ncncc(C#N)c(CSC(NC)=NCC)n)c00000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
@@ -721,10 +721,10 @@
     <t>OCCN(C@CC(C)(C)C)C(C@NCcccc(C=C(C)N=CO)cc)C00000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>OC(C)C(C@NS@@ccccc(-ccccc(N)nc(Cl)ncc)c)[N+]0000000000000000000000000000000000000000000000000000000000000000000000000000</t>
-  </si>
-  <si>
-    <t>/C=C(\S@@NC=Ncccc(Cl)ccS)ccccccS0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>OC(C)C(C@NS@@ccccc(-ccccc(N)nc(l)ncc)c)[N+]00000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+  </si>
+  <si>
+    <t>/C=C(\S@@NC=Ncccc(l)ccS)ccccccS00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>cncc(-ccccc(C(cccccc)C@n(C)[c+](=N)n)c)cc0000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
@@ -736,7 +736,7 @@
     <t>C=CC[N+]CCOC(C[C-]@=O)C([C-]@=O)NC@C000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>Occcc(/C=C(\)cccOHccOHc)cc0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>Occcc(/C=C(\)ccc&amp;cc&amp;c)cc000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>NC@ON(CC([C-]@=O)[N+])C=O00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
@@ -748,7 +748,7 @@
     <t>OCCN(C@C(NC@C(F)CC)C(C)(C)C)C(C@NCcccc(C=C(C)N=CS)cc)C000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>C=NN=NNcccc(Cl)ccCNC@CNC@C(NCC(F)(F)cccccn=O)=NC=CCl00000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>C=NN=NNcccc(l)ccCNC@CNC@C(NCC(F)(F)cccccn=O)=NC=Cl0000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>C(=C(C(/)=C/ccccc(C)cCCC)\C)/C=C/C(=C(\)[C-]@=O)C00000000000000000000000000000000000000000000000000000000000000000000000</t>
@@ -790,10 +790,10 @@
     <t>ccc(S@@N)cccCCSC=NC=C(C@n[c+](=N)n)N000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>/C=C(\C@C@N(C)C)ccc(C@NCC(C)[N+](Ccccc(F)cc)CCC)c(Cl)ccNC000000000000000000000000000000000000000000000000000000000000000</t>
-  </si>
-  <si>
-    <t>C=C(NCC@NS@=O)C(Cl)=C(cccccc)S000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>/C=C(\C@C@N(C)C)ccc(C@NCC(C)[N+](Ccccc(F)cc)CCC)c(l)ccNC0000000000000000000000000000000000000000000000000000000000000000</t>
+  </si>
+  <si>
+    <t>C=C(NCC@NS@=O)C(l)=C(cccccc)S0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>Occcc(C)ccO0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
@@ -805,7 +805,7 @@
     <t>OCC(NC=C(/N=C\)C@n[c+](=N)n)OC(COP@@OP@@OP@@=O)CO00000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>C=C(Cl)C@N=C(Cl)CCl00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>C=C(l)C@N=C(l)Cl00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>/C=C(\SCC@Nccccc(c)OCCO)ccccccNCCNC@ccccc(C(F)(F)F)c00000000000000000000000000000000000000000000000000000000000000000000</t>
@@ -814,10 +814,10 @@
     <t>Occcc(/N=N/cccccc[C-]@=O)ccC00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>Occcc(C=COcccOHccOHcC=O)cc0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
-  </si>
-  <si>
-    <t>cccc(-cc([C-]@=O)c(C)ncccc(Cl)cc)cc0000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>Occcc(C=COccc&amp;cc&amp;cC=O)cc000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+  </si>
+  <si>
+    <t>cccc(-cc([C-]@=O)c(C)ncccc(l)cc)cc00000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>OCCNN=C(C)C=CCCCC=O00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
@@ -847,7 +847,7 @@
     <t>ccc(F)c(N)c([C-]@=O)c000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>OCCCOHCOHC[N+]0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>OCCC&amp;C&amp;C[N+]000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>C=NC@C=C(O/C(ccccc(S@@NC)c)=C\)C0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
@@ -865,7 +865,7 @@
     <t>C=CNcnccc(c)N(CCN(C@CC#N)CCC)N=N0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>OCC(N/C=N\cc(NCccccc(Cl)c)ncnc)OC(CSCCC([C-]@=O)[N+])CO00000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>OCC(N/C=N\cc(NCccccc(l)c)ncnc)OC(CSCCC([C-]@=O)[N+])CO000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>/C(=C(/)CCCCCCC)[C-]@=O0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
@@ -877,10 +877,10 @@
     <t>cc(F)cc(-cccc([C-]@=O)cc)ccF00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>OCCCOHC[N+](C/C=C(\)NC=CN=CNC=O)C000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
-  </si>
-  <si>
-    <t>/C=C(\S@@NC=Ncccc(Cl)ccS)Scccccc0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>OCCC&amp;C[N+](C/C=C(\)NC=CN=CNC=O)C0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+  </si>
+  <si>
+    <t>/C=C(\S@@NC=Ncccc(l)ccS)Scccccc00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>C=C(OCCC)C=CNC(C@C)=CC(ccccccS@@C)=C000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
@@ -892,7 +892,7 @@
     <t>OCC([C-]@=O)[N+]00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>OCCCNC@COHCO000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>OCCCNC@C&amp;CO0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>cnc(Ncccc(N(C)C)cc)nc(C=C(C)N=C(C)S)c00000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
@@ -910,22 +910,22 @@
     <t>Occcc(N@=O)ccO0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>Occncc(-ccc(CC([C-]@=O)[N+])cc(Cl)cCl)c000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>Occncc(-ccc(CC([C-]@=O)[N+])cc(l)cl)c00000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>/C(=C(\)C/C=C(/)CCC[C-]@=O)C/C=C(/)C/C=C(/)CCCCC000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>OccOHc(S@@=O)cccC@ccccccC=O000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>Occ&amp;c(S@@=O)cccC@ccccccC=O0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>OS(cccc(C=NC(cccncc)=C(cccc(F)cc)N)cc)C000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>cnc(Ncccc([C-]@=O)cc)nccC/N=C(/cc(F)ccccF)ccc(Cl)ccc0000000000000000000000000000000000000000000000000000000000000000000-</t>
-  </si>
-  <si>
-    <t>ccc(C=NSC(C)=CC@N=[C+](=N)=NCccc(Cl)c(NC@C)c(C)c)cccOC000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>cnc(Ncccc([C-]@=O)cc)nccC/N=C(/cc(F)ccccF)ccc(l)ccc00000000000000000000000000000000000000000000000000000000000000000000-</t>
+  </si>
+  <si>
+    <t>ccc(C=NSC(C)=CC@N=[C+](=N)=NCccc(l)c(NC@C)c(C)c)cccOC0000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>C=CC(C@NCCCCC([N+])CC)NC@N(CCS@@cccccc)C@NC00000000000000000000000000000000000000000000000000000000000000000000000000000</t>
@@ -937,7 +937,7 @@
     <t>ccc(-ccc(C=NN=C(C)O)cccC)cccC@NCCCC0000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>OCCOC(OCCCOHCOHC[N+]C)COHCOHCO000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>OCCOC(OCCC&amp;C&amp;C[N+]C)C&amp;C&amp;CO0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>C(=C(\C)CC(C[C-]@=O)C([C-]@=O)[N+]C)/C=C(\)C([C-]@=O)C000000000000000000000000000000000000000000000000000000000000000000</t>
@@ -955,13 +955,13 @@
     <t>ccc(C)c(OCCCC([C-]@=O)(C)C)ccC000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>Occcc(C=C(Br)C(OC[C-]@=O)=C([C-]@=O)S)cc00000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>Occcc(C=C(*)C(OC[C-]@=O)=C([C-]@=O)S)cc000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>ccc(CCC([C-]@=O)[N+])cccNC@C@N000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>C=C(NC@Nccccc(Cl)cCl)N(cccccc)N=CC(C)(C)C0000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>C=C(NC@Nccccc(l)cl)N(cccccc)N=CC(C)(C)C000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>ccc(NC@cccc(C)c(-ccccc(c)ON=CCCC[N+]CC)c)cc(NCCOCC)c00000000000000000000000000000000000000000000000000000000000000000000</t>
@@ -970,7 +970,7 @@
     <t>OccccccO0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>/N=C\C=CN(COC(COP@@OP@@=O)COHCO)C@N0000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>/N=C\C=CN(COC(COP@@OP@@=O)C&amp;CO)C@N00000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>Ncnc(OCCCCCCC)c(N=O)c(N)n00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
@@ -988,16 +988,16 @@
     <t>OCC(C)(C)[N+](CC=NSC(NC=NC(C)=CN/C=N\C=C/C=CNN=C)=C)CC000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>cnc(C@NC)cc(Occcc(NC@Ncccc(Cl)c(C(F)(F)F)c)cc)c0000000000000000000000000000000000000000000000000000000000000000000000000</t>
-  </si>
-  <si>
-    <t>C=C(C)N(ccc(C@NC)cccC)C@C(Br)=COCcccc(F)ccF00000000000000000000000000000000000000000000000000000000000000000000000000000</t>
-  </si>
-  <si>
-    <t>OCC(OP@@=O)COHC(OP@@=O)C(OP@@=O)COP@@=O000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
-  </si>
-  <si>
-    <t>CC(C)CC(Cl)[C-]@=O000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>cnc(C@NC)cc(Occcc(NC@Ncccc(l)c(C(F)(F)F)c)cc)c00000000000000000000000000000000000000000000000000000000000000000000000000</t>
+  </si>
+  <si>
+    <t>C=C(C)N(ccc(C@NC)cccC)C@C(*)=COCcccc(F)ccF000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+  </si>
+  <si>
+    <t>OCC(OP@@=O)C&amp;C(OP@@=O)C(OP@@=O)COP@@=O0000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+  </si>
+  <si>
+    <t>CC(C)CC(l)[C-]@=O0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>cnc(N)cc(Ncccc(S@@N)cc)n000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
@@ -1021,7 +1021,7 @@
     <t>OCCN(C@C(NC@C(NC@C)Ccccccc)C(C)(C)C)C(C@NCcccc(C=C(C)N=CS)cc)C0000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>ccc(CS[C+](=N)=N)cc(Cl)cOCCCC0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>ccc(CS[C+](=N)=N)cc(l)cOCCCC00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>C=C(ccncc(C@OC)c)OC=CC@N/C=C\0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
@@ -1054,7 +1054,7 @@
     <t>OC(C(NC@ccccc(c)N(C)S@@C(C)(C)CNC=CCC)Ccccccc)CC@N(Ccccccc)CC[N+]0000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>OCCCOHCOHCCCC[N+]0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>OCCC&amp;C&amp;CCCC[N+]000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>cnc(Ncccc([C-]@=O)cc)nc(NccccccOC(F)(F)F)c000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
@@ -1063,7 +1063,7 @@
     <t>OCCN(C@CC(C)(C)C)C(C@NCcccc(C=CN=CO)cc)C00000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>cnc(N)c(CCccccc(Cl)c)cc0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>cnc(N)c(CCccccc(l)c)cc00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>C=CNcnccc(c)N(CCC[N+]CC)/C(C)=N\0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
@@ -1072,7 +1072,7 @@
     <t>OCC=C(SC)SN=CSC000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>ccc(C=C(Br)C(OC[C-]@=O)=C([C-]@=O)S)cc(NCCC(C)(C)CC(C)(C)C)c000000000000000000000000000000000000000000000000000000000000</t>
+    <t>ccc(C=C(*)C(OC[C-]@=O)=C([C-]@=O)S)cc(NCCC(C)(C)CC(C)(C)C)c0000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>OCCCOCCC([C-]@=O)(CC([C-]@=O)[N+])OC000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
@@ -1108,7 +1108,7 @@
     <t>ccc(C(cccc(N(C)C)cc)cccc(N(C)C)cc)cccN(C)C000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>C=C(cnccc(c)C(ccc(NC@cncc(Cl)cc)cccO)n[c+](=N)OC)C=CCO000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>C=C(cnccc(c)C(ccc(NC@cncc(l)cc)cccO)n[c+](=N)OC)C=CCO0000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>OCCN(C@C(NC@C)C(C)(C)C)C(C@NCcccc(C=C(C)N=CS)cc)C00000000000000000000000000000000000000000000000000000000000000000000000</t>
@@ -1132,13 +1132,13 @@
     <t>OCC[N+](C)(C)C0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>CC@N(C)CC(C@OCC)=CCl0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>CC@N(C)CC(C@OCC)=Cl00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>cccc(NN=C(C@N)C(C)=N)cc0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>Occ(Cl)cc(-ccc(Cl)cOHc(Cl)c)ccCl0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>Occ(l)cc(-ccc(l)c&amp;c(l)c)ccl000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>cccc(C(cccccc)C@n(C)[c+](=N)n)cc0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
@@ -1147,7 +1147,7 @@
     <t>cnccc(c)C([C-]@=O)=C(NC@[C-]@=O)S000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>OCCCOHCOHC[N+]C000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>OCCC&amp;C&amp;C[N+]C00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>CC(C)CC@[C-]@=O000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
@@ -1156,13 +1156,13 @@
     <t>Occccc(OCCCCNC@C(NC@OC(C)(C)C)Ccccc(OC([C-]@=O)[C-]@=O)cc)cC@OC000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>ccccc(S@@NCCCC[C-]@=O)ccc(Br)cc00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>ccccc(S@@NCCCC[C-]@=O)ccc(*)cc000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>OCC(N/C=N\cc(N)ncnc)OC(COP@@OP@@OP@@=O)CO0000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>C=NN(ccccc(Cl)c)C=CC@N/C(SC(C@N)C)=N\00000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>C=NN(ccccc(l)c)C=CC@N/C(SC(C@N)C)=N\000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>Occc(C@ccccccF)cc(N@=O)cO00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
@@ -1189,7 +1189,7 @@
     <t>cccc(CCCCC@NC@CC)cc00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>Occcc(C=CC@ccOHcc(Cl)ccO)ccO00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>Occcc(C=CC@cc&amp;cc(l)ccO)ccO0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>OC(C(NC@CNC@N(Cccccc(OC)c)C)Ccccccc)C[N+]Cccccc(N(C)C)c00000000000000000000000000000000000000000000000000000000000000000</t>
@@ -1198,10 +1198,10 @@
     <t>cccc(C=C(cccccc)N(CC[C-]@=O)cccc(CCC)cc)cc000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>OCCN(C@CN(C@C)CCOHC)C(C@NCcccc(C=C(C)N=CS)cc)C00000000000000000000000000000000000000000000000000000000000000000000000000</t>
-  </si>
-  <si>
-    <t>/C=N/cc(Nccccc(Cl)c)nc(NCCCCCC[N+])ncNCC00000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>OCCN(C@CN(C@C)CC&amp;C)C(C@NCcccc(C=C(C)N=CS)cc)C000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+  </si>
+  <si>
+    <t>/C=N/cc(Nccccc(l)c)nc(NCCCCCC[N+])ncNCC000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>N=[c+]nC@C=C(N(C)C(SC[C-]@=O)=N)n000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
@@ -1210,7 +1210,7 @@
     <t>Occcc(-cccccc)ccO0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>ccc(-cc([C-]@=O)c(C(C)C)ncccc(Cl)cc)cc(C(C)C)c00000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>ccc(-cc([C-]@=O)c(C(C)C)ncccc(l)cc)cc(C(C)C)c000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>OCCOCCC([C-]@=O)(CC([C-]@=O)[N+])OCCO00000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
@@ -1219,7 +1219,7 @@
     <t>cnc(Nccccc(NCCN(C@C)CCC)c)nc(C=C(C)N=C(NC)S)cC#N000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>Occcc(/C=C(\)ccccc([C-]@=O)c)c(Cl)c0000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>Occcc(/C=C(\)ccccc([C-]@=O)c)c(l)c00000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>C=NC(cccc(F)cc)=C(cnc(N)ncc)NCCC[N+]CC0000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
@@ -1234,7 +1234,7 @@
     <t>/C(=C(/)CCCCCCCCC[C-]@=O)CC000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>cc(Cl)c(Cl)cc(OC[C-]@=O)cCl000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>cc(l)c(l)cc(OC[C-]@=O)cl000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>OCC([C-]@=O)Ncccc(N@=O)ccN@=O0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
@@ -1252,7 +1252,7 @@
     <t>Occcc(C)c(N(C@C)C=CN(C@C)cccccc)c000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>Occcc(C=CC@ccOHccOHccO)cc00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>Occcc(C=CC@cc&amp;cc&amp;ccO)cc0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>Occ(C)c(C)cc(cC)CCC(C)(COcccc(CCSC@NC=O)cc)O0000000000000000000000000000000000000000000000000000000000000000000000000000</t>
@@ -1261,13 +1261,13 @@
     <t>NC=NC=C(N=C(SCC@NC)N)C@N000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>OcccOHcc(c)O/C(cccccc)=C(/)C=O000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
-  </si>
-  <si>
-    <t>OCCCOHCOHCOHC[N+]0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
-  </si>
-  <si>
-    <t>ccccc(c)N=C(C(OC@Ncccc(Cl)c(Cl)c)C)N000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>Occc&amp;cc(c)O/C(cccccc)=C(/)C=O0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+  </si>
+  <si>
+    <t>OCCC&amp;C&amp;C&amp;C[N+]0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+  </si>
+  <si>
+    <t>ccccc(c)N=C(C(OC@Ncccc(l)c(l)c)C)N00000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>Occcc(CC[N+])ccCC0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
@@ -1276,13 +1276,13 @@
     <t>Occcc(F)ccO0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>ccc(C@NC(C)=C(C[C-]@=O)ccc(OC)ccc)cccCl000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>ccc(C@NC(C)=C(C[C-]@=O)ccc(OC)ccc)cccl0000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>C=CNcnccc(c)N(CCCCCCC)/C(CNS@@C)=N\0000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
-    <t>Occcc(C=CC@ccOHcc(OC)ccO)ccO00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
+    <t>Occcc(C=CC@cc&amp;cc(OC)ccO)ccO000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</t>
   </si>
   <si>
     <t>cnc(Ncccc([C-]@=O)cc)nc(NccccccC(F)(F)F)c0000000000000000000000000000000000000000000000000000000000000000000000000000000</t>

</xml_diff>